<commit_message>
Added Integrity column to filter good data
</commit_message>
<xml_diff>
--- a/data/robot_1_data.xlsx
+++ b/data/robot_1_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F384"/>
+  <dimension ref="A1:G384"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,6 +463,11 @@
           <t>Station2_Inverter1_MinusWire</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Integrity</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -483,6 +488,9 @@
       <c r="F2" t="n">
         <v>27.849</v>
       </c>
+      <c r="G2" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -502,6 +510,9 @@
       </c>
       <c r="F3" t="n">
         <v>27.5</v>
+      </c>
+      <c r="G3" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -517,6 +528,9 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -531,6 +545,9 @@
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -550,6 +567,9 @@
       </c>
       <c r="F6" t="n">
         <v>27.1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -571,6 +591,9 @@
       <c r="F7" t="n">
         <v>27.1</v>
       </c>
+      <c r="G7" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -585,6 +608,9 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -599,6 +625,9 @@
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
+      <c r="G9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -619,6 +648,9 @@
       <c r="F10" t="n">
         <v>27.6</v>
       </c>
+      <c r="G10" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -639,6 +671,9 @@
       <c r="F11" t="n">
         <v>27.6</v>
       </c>
+      <c r="G11" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -653,6 +688,9 @@
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
+      <c r="G12" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -673,6 +711,9 @@
       <c r="F13" t="n">
         <v>27.6</v>
       </c>
+      <c r="G13" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -693,6 +734,9 @@
       <c r="F14" t="n">
         <v>27.6</v>
       </c>
+      <c r="G14" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -713,6 +757,9 @@
       <c r="F15" t="n">
         <v>27.6</v>
       </c>
+      <c r="G15" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -733,6 +780,9 @@
       <c r="F16" t="n">
         <v>27.6</v>
       </c>
+      <c r="G16" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -753,6 +803,9 @@
       <c r="F17" t="n">
         <v>27.6</v>
       </c>
+      <c r="G17" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -773,6 +826,9 @@
       <c r="F18" t="n">
         <v>27.6</v>
       </c>
+      <c r="G18" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -787,6 +843,9 @@
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
+      <c r="G19" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -801,6 +860,9 @@
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
+      <c r="G20" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -821,6 +883,9 @@
       <c r="F21" t="n">
         <v>25.4</v>
       </c>
+      <c r="G21" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -841,6 +906,9 @@
       <c r="F22" t="n">
         <v>25.4</v>
       </c>
+      <c r="G22" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -855,6 +923,9 @@
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
+      <c r="G23" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -869,6 +940,9 @@
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
+      <c r="G24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -889,6 +963,9 @@
       <c r="F25" t="n">
         <v>27.3</v>
       </c>
+      <c r="G25" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -909,6 +986,9 @@
       <c r="F26" t="n">
         <v>27.3</v>
       </c>
+      <c r="G26" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -923,6 +1003,9 @@
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
+      <c r="G27" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -943,6 +1026,9 @@
       <c r="F28" t="n">
         <v>25.8</v>
       </c>
+      <c r="G28" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -963,6 +1049,9 @@
       <c r="F29" t="n">
         <v>25.8</v>
       </c>
+      <c r="G29" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -983,6 +1072,9 @@
       <c r="F30" t="n">
         <v>25.8</v>
       </c>
+      <c r="G30" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -999,6 +1091,9 @@
       </c>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
+      <c r="G31" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1013,6 +1108,9 @@
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
+      <c r="G32" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1033,6 +1131,9 @@
       <c r="F33" t="n">
         <v>27.6</v>
       </c>
+      <c r="G33" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1053,6 +1154,9 @@
       <c r="F34" t="n">
         <v>27.6</v>
       </c>
+      <c r="G34" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1067,6 +1171,9 @@
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
+      <c r="G35" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1087,6 +1194,9 @@
       <c r="F36" t="n">
         <v>26.6</v>
       </c>
+      <c r="G36" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1107,6 +1217,9 @@
       <c r="F37" t="n">
         <v>26.6</v>
       </c>
+      <c r="G37" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1121,6 +1234,9 @@
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr"/>
+      <c r="G38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1135,6 +1251,9 @@
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr"/>
+      <c r="G39" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -1155,6 +1274,9 @@
       <c r="F40" t="n">
         <v>26.8</v>
       </c>
+      <c r="G40" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -1175,6 +1297,9 @@
       <c r="F41" t="n">
         <v>26.8</v>
       </c>
+      <c r="G41" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -1195,6 +1320,9 @@
       <c r="F42" t="n">
         <v>26.8</v>
       </c>
+      <c r="G42" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1215,6 +1343,9 @@
       <c r="F43" t="n">
         <v>24.6</v>
       </c>
+      <c r="G43" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1235,6 +1366,9 @@
       <c r="F44" t="n">
         <v>25.6</v>
       </c>
+      <c r="G44" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -1249,6 +1383,9 @@
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr"/>
+      <c r="G45" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -1269,6 +1406,9 @@
       <c r="F46" t="n">
         <v>25.6</v>
       </c>
+      <c r="G46" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -1283,6 +1423,9 @@
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr"/>
+      <c r="G47" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -1297,6 +1440,9 @@
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr"/>
+      <c r="G48" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -1317,6 +1463,9 @@
       <c r="F49" t="n">
         <v>25.3</v>
       </c>
+      <c r="G49" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -1337,6 +1486,9 @@
       <c r="F50" t="n">
         <v>25.3</v>
       </c>
+      <c r="G50" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -1351,6 +1503,9 @@
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr"/>
+      <c r="G51" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -1371,6 +1526,9 @@
       <c r="F52" t="n">
         <v>26.1</v>
       </c>
+      <c r="G52" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -1391,6 +1549,9 @@
       <c r="F53" t="n">
         <v>26.1</v>
       </c>
+      <c r="G53" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -1405,6 +1566,9 @@
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr"/>
+      <c r="G54" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -1419,6 +1583,9 @@
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr"/>
+      <c r="G55" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -1439,6 +1606,9 @@
       <c r="F56" t="n">
         <v>24.4</v>
       </c>
+      <c r="G56" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -1459,6 +1629,9 @@
       <c r="F57" t="n">
         <v>24.4</v>
       </c>
+      <c r="G57" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -1473,6 +1646,9 @@
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr"/>
+      <c r="G58" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -1489,6 +1665,9 @@
       <c r="F59" t="n">
         <v>26</v>
       </c>
+      <c r="G59" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -1509,6 +1688,9 @@
       <c r="F60" t="n">
         <v>26</v>
       </c>
+      <c r="G60" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -1529,6 +1711,9 @@
       <c r="F61" t="n">
         <v>26</v>
       </c>
+      <c r="G61" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -1549,6 +1734,9 @@
       <c r="F62" t="n">
         <v>26</v>
       </c>
+      <c r="G62" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -1569,6 +1757,9 @@
       <c r="F63" t="n">
         <v>26</v>
       </c>
+      <c r="G63" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -1589,6 +1780,9 @@
       <c r="F64" t="n">
         <v>25.1</v>
       </c>
+      <c r="G64" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -1609,6 +1803,9 @@
       <c r="F65" t="n">
         <v>25.1</v>
       </c>
+      <c r="G65" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -1629,6 +1826,9 @@
       <c r="F66" t="n">
         <v>25.1</v>
       </c>
+      <c r="G66" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -1649,6 +1849,9 @@
       <c r="F67" t="n">
         <v>25.1</v>
       </c>
+      <c r="G67" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -1669,6 +1872,9 @@
       <c r="F68" t="n">
         <v>25.1</v>
       </c>
+      <c r="G68" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -1689,6 +1895,9 @@
       <c r="F69" t="n">
         <v>25.1</v>
       </c>
+      <c r="G69" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -1709,6 +1918,9 @@
       <c r="F70" t="n">
         <v>25.1</v>
       </c>
+      <c r="G70" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -1729,6 +1941,9 @@
       <c r="F71" t="n">
         <v>25.1</v>
       </c>
+      <c r="G71" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -1749,6 +1964,9 @@
       <c r="F72" t="n">
         <v>25.1</v>
       </c>
+      <c r="G72" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -1763,6 +1981,9 @@
       <c r="D73" t="inlineStr"/>
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr"/>
+      <c r="G73" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -1783,6 +2004,9 @@
       <c r="F74" t="n">
         <v>24.6</v>
       </c>
+      <c r="G74" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -1803,6 +2027,9 @@
       <c r="F75" t="n">
         <v>24.6</v>
       </c>
+      <c r="G75" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -1817,6 +2044,9 @@
       <c r="D76" t="inlineStr"/>
       <c r="E76" t="inlineStr"/>
       <c r="F76" t="inlineStr"/>
+      <c r="G76" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -1833,6 +2063,9 @@
         <v>25.8</v>
       </c>
       <c r="F77" t="inlineStr"/>
+      <c r="G77" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -1853,6 +2086,9 @@
       <c r="F78" t="n">
         <v>26</v>
       </c>
+      <c r="G78" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -1873,6 +2109,9 @@
       <c r="F79" t="n">
         <v>26</v>
       </c>
+      <c r="G79" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -1887,6 +2126,9 @@
       <c r="D80" t="inlineStr"/>
       <c r="E80" t="inlineStr"/>
       <c r="F80" t="inlineStr"/>
+      <c r="G80" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -1901,6 +2143,9 @@
       <c r="D81" t="inlineStr"/>
       <c r="E81" t="inlineStr"/>
       <c r="F81" t="inlineStr"/>
+      <c r="G81" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -1921,6 +2166,9 @@
       <c r="F82" t="n">
         <v>25.8</v>
       </c>
+      <c r="G82" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -1941,6 +2189,9 @@
       <c r="F83" t="n">
         <v>25.8</v>
       </c>
+      <c r="G83" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -1955,6 +2206,9 @@
       <c r="D84" t="inlineStr"/>
       <c r="E84" t="inlineStr"/>
       <c r="F84" t="inlineStr"/>
+      <c r="G84" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -1975,6 +2229,9 @@
       <c r="F85" t="n">
         <v>24.9</v>
       </c>
+      <c r="G85" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -1989,6 +2246,9 @@
       <c r="D86" t="inlineStr"/>
       <c r="E86" t="inlineStr"/>
       <c r="F86" t="inlineStr"/>
+      <c r="G86" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -2003,6 +2263,9 @@
       <c r="D87" t="inlineStr"/>
       <c r="E87" t="inlineStr"/>
       <c r="F87" t="inlineStr"/>
+      <c r="G87" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -2017,6 +2280,9 @@
       <c r="D88" t="inlineStr"/>
       <c r="E88" t="inlineStr"/>
       <c r="F88" t="inlineStr"/>
+      <c r="G88" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -2037,6 +2303,9 @@
       <c r="F89" t="n">
         <v>26</v>
       </c>
+      <c r="G89" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -2057,6 +2326,9 @@
       <c r="F90" t="n">
         <v>26</v>
       </c>
+      <c r="G90" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -2071,6 +2343,9 @@
       <c r="D91" t="inlineStr"/>
       <c r="E91" t="inlineStr"/>
       <c r="F91" t="inlineStr"/>
+      <c r="G91" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -2085,6 +2360,9 @@
       <c r="D92" t="inlineStr"/>
       <c r="E92" t="inlineStr"/>
       <c r="F92" t="inlineStr"/>
+      <c r="G92" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -2105,6 +2383,9 @@
       <c r="F93" t="n">
         <v>26</v>
       </c>
+      <c r="G93" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -2125,6 +2406,9 @@
       <c r="F94" t="n">
         <v>26</v>
       </c>
+      <c r="G94" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -2139,6 +2423,9 @@
       <c r="D95" t="inlineStr"/>
       <c r="E95" t="inlineStr"/>
       <c r="F95" t="inlineStr"/>
+      <c r="G95" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -2153,6 +2440,9 @@
       <c r="D96" t="inlineStr"/>
       <c r="E96" t="inlineStr"/>
       <c r="F96" t="inlineStr"/>
+      <c r="G96" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -2173,6 +2463,9 @@
       <c r="F97" t="n">
         <v>26.6</v>
       </c>
+      <c r="G97" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -2193,6 +2486,9 @@
       <c r="F98" t="n">
         <v>26.6</v>
       </c>
+      <c r="G98" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -2213,6 +2509,9 @@
       <c r="F99" t="n">
         <v>26.6</v>
       </c>
+      <c r="G99" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -2233,6 +2532,9 @@
       <c r="F100" t="n">
         <v>26.6</v>
       </c>
+      <c r="G100" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -2253,6 +2555,9 @@
       <c r="F101" t="n">
         <v>26.6</v>
       </c>
+      <c r="G101" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -2273,6 +2578,9 @@
       <c r="F102" t="n">
         <v>26.6</v>
       </c>
+      <c r="G102" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -2287,6 +2595,9 @@
       <c r="D103" t="inlineStr"/>
       <c r="E103" t="inlineStr"/>
       <c r="F103" t="inlineStr"/>
+      <c r="G103" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -2301,6 +2612,9 @@
       <c r="D104" t="inlineStr"/>
       <c r="E104" t="inlineStr"/>
       <c r="F104" t="inlineStr"/>
+      <c r="G104" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -2321,6 +2635,9 @@
       <c r="F105" t="n">
         <v>26</v>
       </c>
+      <c r="G105" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -2341,6 +2658,9 @@
       <c r="F106" t="n">
         <v>26</v>
       </c>
+      <c r="G106" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -2355,6 +2675,9 @@
       <c r="D107" t="inlineStr"/>
       <c r="E107" t="inlineStr"/>
       <c r="F107" t="inlineStr"/>
+      <c r="G107" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -2369,6 +2692,9 @@
       <c r="D108" t="inlineStr"/>
       <c r="E108" t="inlineStr"/>
       <c r="F108" t="inlineStr"/>
+      <c r="G108" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -2389,6 +2715,9 @@
       <c r="F109" t="n">
         <v>25.3</v>
       </c>
+      <c r="G109" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -2409,6 +2738,9 @@
       <c r="F110" t="n">
         <v>25.3</v>
       </c>
+      <c r="G110" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -2423,6 +2755,9 @@
       <c r="D111" t="inlineStr"/>
       <c r="E111" t="inlineStr"/>
       <c r="F111" t="inlineStr"/>
+      <c r="G111" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -2443,6 +2778,9 @@
       <c r="F112" t="n">
         <v>25.3</v>
       </c>
+      <c r="G112" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -2463,6 +2801,9 @@
       <c r="F113" t="n">
         <v>25.3</v>
       </c>
+      <c r="G113" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -2479,6 +2820,9 @@
         <v>23.8</v>
       </c>
       <c r="F114" t="inlineStr"/>
+      <c r="G114" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -2493,6 +2837,9 @@
       <c r="D115" t="inlineStr"/>
       <c r="E115" t="inlineStr"/>
       <c r="F115" t="inlineStr"/>
+      <c r="G115" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -2513,6 +2860,9 @@
       <c r="F116" t="n">
         <v>26.3</v>
       </c>
+      <c r="G116" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -2533,6 +2883,9 @@
       <c r="F117" t="n">
         <v>26.3</v>
       </c>
+      <c r="G117" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -2547,6 +2900,9 @@
       <c r="D118" t="inlineStr"/>
       <c r="E118" t="inlineStr"/>
       <c r="F118" t="inlineStr"/>
+      <c r="G118" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -2561,6 +2917,9 @@
       <c r="D119" t="inlineStr"/>
       <c r="E119" t="inlineStr"/>
       <c r="F119" t="inlineStr"/>
+      <c r="G119" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -2581,6 +2940,9 @@
       <c r="F120" t="n">
         <v>26.1</v>
       </c>
+      <c r="G120" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -2601,6 +2963,9 @@
       <c r="F121" t="n">
         <v>26.1</v>
       </c>
+      <c r="G121" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -2615,6 +2980,9 @@
       <c r="D122" t="inlineStr"/>
       <c r="E122" t="inlineStr"/>
       <c r="F122" t="inlineStr"/>
+      <c r="G122" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -2635,6 +3003,9 @@
       <c r="F123" t="n">
         <v>26</v>
       </c>
+      <c r="G123" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -2655,6 +3026,9 @@
       <c r="F124" t="n">
         <v>26</v>
       </c>
+      <c r="G124" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
@@ -2675,6 +3049,9 @@
       <c r="F125" t="n">
         <v>25.8</v>
       </c>
+      <c r="G125" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -2695,6 +3072,9 @@
       <c r="F126" t="n">
         <v>25.8</v>
       </c>
+      <c r="G126" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -2715,6 +3095,9 @@
       <c r="F127" t="n">
         <v>25.8</v>
       </c>
+      <c r="G127" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
@@ -2735,6 +3118,9 @@
       <c r="F128" t="n">
         <v>25.6</v>
       </c>
+      <c r="G128" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
@@ -2755,6 +3141,9 @@
       <c r="F129" t="n">
         <v>25.8</v>
       </c>
+      <c r="G129" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
@@ -2775,6 +3164,9 @@
       <c r="F130" t="n">
         <v>25.8</v>
       </c>
+      <c r="G130" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
@@ -2789,6 +3181,9 @@
       <c r="D131" t="inlineStr"/>
       <c r="E131" t="inlineStr"/>
       <c r="F131" t="inlineStr"/>
+      <c r="G131" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
@@ -2809,6 +3204,9 @@
       <c r="F132" t="n">
         <v>25.8</v>
       </c>
+      <c r="G132" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
@@ -2823,6 +3221,9 @@
       <c r="D133" t="inlineStr"/>
       <c r="E133" t="inlineStr"/>
       <c r="F133" t="inlineStr"/>
+      <c r="G133" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
@@ -2837,6 +3238,9 @@
       <c r="D134" t="inlineStr"/>
       <c r="E134" t="inlineStr"/>
       <c r="F134" t="inlineStr"/>
+      <c r="G134" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
@@ -2857,6 +3261,9 @@
       <c r="F135" t="n">
         <v>25.3</v>
       </c>
+      <c r="G135" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
@@ -2877,6 +3284,9 @@
       <c r="F136" t="n">
         <v>25.3</v>
       </c>
+      <c r="G136" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
@@ -2891,6 +3301,9 @@
       <c r="D137" t="inlineStr"/>
       <c r="E137" t="inlineStr"/>
       <c r="F137" t="inlineStr"/>
+      <c r="G137" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
@@ -2905,6 +3318,9 @@
       <c r="D138" t="inlineStr"/>
       <c r="E138" t="inlineStr"/>
       <c r="F138" t="inlineStr"/>
+      <c r="G138" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
@@ -2925,6 +3341,9 @@
       <c r="F139" t="n">
         <v>26</v>
       </c>
+      <c r="G139" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
@@ -2945,6 +3364,9 @@
       <c r="F140" t="n">
         <v>26</v>
       </c>
+      <c r="G140" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
@@ -2959,6 +3381,9 @@
       <c r="D141" t="inlineStr"/>
       <c r="E141" t="inlineStr"/>
       <c r="F141" t="inlineStr"/>
+      <c r="G141" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
@@ -2979,6 +3404,9 @@
       <c r="F142" t="n">
         <v>25.4</v>
       </c>
+      <c r="G142" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
@@ -2999,6 +3427,9 @@
       <c r="F143" t="n">
         <v>25.4</v>
       </c>
+      <c r="G143" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
@@ -3013,6 +3444,9 @@
       <c r="D144" t="inlineStr"/>
       <c r="E144" t="inlineStr"/>
       <c r="F144" t="inlineStr"/>
+      <c r="G144" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
@@ -3027,6 +3461,9 @@
       <c r="D145" t="inlineStr"/>
       <c r="E145" t="inlineStr"/>
       <c r="F145" t="inlineStr"/>
+      <c r="G145" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
@@ -3047,6 +3484,9 @@
       <c r="F146" t="n">
         <v>24.9</v>
       </c>
+      <c r="G146" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
@@ -3067,6 +3507,9 @@
       <c r="F147" t="n">
         <v>24.9</v>
       </c>
+      <c r="G147" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
@@ -3081,6 +3524,9 @@
       <c r="D148" t="inlineStr"/>
       <c r="E148" t="inlineStr"/>
       <c r="F148" t="inlineStr"/>
+      <c r="G148" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
@@ -3095,6 +3541,9 @@
       <c r="D149" t="inlineStr"/>
       <c r="E149" t="inlineStr"/>
       <c r="F149" t="inlineStr"/>
+      <c r="G149" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
@@ -3115,6 +3564,9 @@
       <c r="F150" t="n">
         <v>23.7</v>
       </c>
+      <c r="G150" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
@@ -3135,6 +3587,9 @@
       <c r="F151" t="n">
         <v>23.7</v>
       </c>
+      <c r="G151" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
@@ -3149,6 +3604,9 @@
       <c r="D152" t="inlineStr"/>
       <c r="E152" t="inlineStr"/>
       <c r="F152" t="inlineStr"/>
+      <c r="G152" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
@@ -3163,6 +3621,9 @@
       <c r="D153" t="inlineStr"/>
       <c r="E153" t="inlineStr"/>
       <c r="F153" t="inlineStr"/>
+      <c r="G153" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
@@ -3183,6 +3644,9 @@
       <c r="F154" t="n">
         <v>24</v>
       </c>
+      <c r="G154" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
@@ -3203,6 +3667,9 @@
       <c r="F155" t="n">
         <v>25.6</v>
       </c>
+      <c r="G155" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
@@ -3223,6 +3690,9 @@
       <c r="F156" t="n">
         <v>25.6</v>
       </c>
+      <c r="G156" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
@@ -3243,6 +3713,9 @@
       <c r="F157" t="n">
         <v>25.6</v>
       </c>
+      <c r="G157" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
@@ -3257,6 +3730,9 @@
       <c r="D158" t="inlineStr"/>
       <c r="E158" t="inlineStr"/>
       <c r="F158" t="inlineStr"/>
+      <c r="G158" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
@@ -3271,6 +3747,9 @@
       <c r="D159" t="inlineStr"/>
       <c r="E159" t="inlineStr"/>
       <c r="F159" t="inlineStr"/>
+      <c r="G159" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
@@ -3291,6 +3770,9 @@
       <c r="F160" t="n">
         <v>26.6</v>
       </c>
+      <c r="G160" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
@@ -3311,6 +3793,9 @@
       <c r="F161" t="n">
         <v>26.6</v>
       </c>
+      <c r="G161" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
@@ -3331,6 +3816,9 @@
       <c r="F162" t="n">
         <v>26.6</v>
       </c>
+      <c r="G162" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
@@ -3351,6 +3839,9 @@
       <c r="F163" t="n">
         <v>26.6</v>
       </c>
+      <c r="G163" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
@@ -3371,6 +3862,9 @@
       <c r="F164" t="n">
         <v>26.6</v>
       </c>
+      <c r="G164" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
@@ -3391,6 +3885,9 @@
       <c r="F165" t="n">
         <v>26.6</v>
       </c>
+      <c r="G165" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
@@ -3411,6 +3908,9 @@
       <c r="F166" t="n">
         <v>26.6</v>
       </c>
+      <c r="G166" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="n">
@@ -3431,6 +3931,9 @@
       <c r="F167" t="n">
         <v>26.6</v>
       </c>
+      <c r="G167" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="n">
@@ -3445,6 +3948,9 @@
       <c r="D168" t="inlineStr"/>
       <c r="E168" t="inlineStr"/>
       <c r="F168" t="inlineStr"/>
+      <c r="G168" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
@@ -3459,6 +3965,9 @@
       <c r="D169" t="inlineStr"/>
       <c r="E169" t="inlineStr"/>
       <c r="F169" t="inlineStr"/>
+      <c r="G169" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="n">
@@ -3479,6 +3988,9 @@
       <c r="F170" t="n">
         <v>26.1</v>
       </c>
+      <c r="G170" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
@@ -3499,6 +4011,9 @@
       <c r="F171" t="n">
         <v>26.1</v>
       </c>
+      <c r="G171" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="n">
@@ -3519,6 +4034,9 @@
       <c r="F172" t="n">
         <v>20.8</v>
       </c>
+      <c r="G172" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="n">
@@ -3533,6 +4051,9 @@
       <c r="D173" t="inlineStr"/>
       <c r="E173" t="inlineStr"/>
       <c r="F173" t="inlineStr"/>
+      <c r="G173" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="n">
@@ -3553,6 +4074,9 @@
       <c r="F174" t="n">
         <v>26.1</v>
       </c>
+      <c r="G174" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="n">
@@ -3573,6 +4097,9 @@
       <c r="F175" t="n">
         <v>26.1</v>
       </c>
+      <c r="G175" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
@@ -3591,6 +4118,9 @@
       <c r="F176" t="n">
         <v>22.2</v>
       </c>
+      <c r="G176" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
@@ -3605,6 +4135,9 @@
       <c r="D177" t="inlineStr"/>
       <c r="E177" t="inlineStr"/>
       <c r="F177" t="inlineStr"/>
+      <c r="G177" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="n">
@@ -3625,6 +4158,9 @@
       <c r="F178" t="n">
         <v>25.4</v>
       </c>
+      <c r="G178" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="n">
@@ -3639,6 +4175,9 @@
       <c r="D179" t="inlineStr"/>
       <c r="E179" t="inlineStr"/>
       <c r="F179" t="inlineStr"/>
+      <c r="G179" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="n">
@@ -3653,6 +4192,9 @@
       <c r="D180" t="inlineStr"/>
       <c r="E180" t="inlineStr"/>
       <c r="F180" t="inlineStr"/>
+      <c r="G180" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
@@ -3669,6 +4211,9 @@
       </c>
       <c r="E181" t="inlineStr"/>
       <c r="F181" t="inlineStr"/>
+      <c r="G181" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="n">
@@ -3689,6 +4234,9 @@
       <c r="F182" t="n">
         <v>26</v>
       </c>
+      <c r="G182" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="n">
@@ -3709,6 +4257,9 @@
       <c r="F183" t="n">
         <v>26</v>
       </c>
+      <c r="G183" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="n">
@@ -3723,6 +4274,9 @@
       <c r="D184" t="inlineStr"/>
       <c r="E184" t="inlineStr"/>
       <c r="F184" t="inlineStr"/>
+      <c r="G184" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="n">
@@ -3737,6 +4291,9 @@
       <c r="D185" t="inlineStr"/>
       <c r="E185" t="inlineStr"/>
       <c r="F185" t="inlineStr"/>
+      <c r="G185" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="n">
@@ -3757,6 +4314,9 @@
       <c r="F186" t="n">
         <v>26.1</v>
       </c>
+      <c r="G186" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="n">
@@ -3777,6 +4337,9 @@
       <c r="F187" t="n">
         <v>26.1</v>
       </c>
+      <c r="G187" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="n">
@@ -3791,6 +4354,9 @@
       <c r="D188" t="inlineStr"/>
       <c r="E188" t="inlineStr"/>
       <c r="F188" t="inlineStr"/>
+      <c r="G188" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="n">
@@ -3805,6 +4371,9 @@
       <c r="D189" t="inlineStr"/>
       <c r="E189" t="inlineStr"/>
       <c r="F189" t="inlineStr"/>
+      <c r="G189" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="n">
@@ -3825,6 +4394,9 @@
       <c r="F190" t="n">
         <v>26.6</v>
       </c>
+      <c r="G190" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="n">
@@ -3845,6 +4417,9 @@
       <c r="F191" t="n">
         <v>26.6</v>
       </c>
+      <c r="G191" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="n">
@@ -3865,6 +4440,9 @@
       <c r="F192" t="n">
         <v>26.6</v>
       </c>
+      <c r="G192" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="n">
@@ -3885,6 +4463,9 @@
       <c r="F193" t="n">
         <v>25.4</v>
       </c>
+      <c r="G193" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="n">
@@ -3905,6 +4486,9 @@
       <c r="F194" t="n">
         <v>26</v>
       </c>
+      <c r="G194" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="n">
@@ -3925,6 +4509,9 @@
       <c r="F195" t="n">
         <v>26</v>
       </c>
+      <c r="G195" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="n">
@@ -3939,6 +4526,9 @@
       <c r="D196" t="inlineStr"/>
       <c r="E196" t="inlineStr"/>
       <c r="F196" t="inlineStr"/>
+      <c r="G196" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="n">
@@ -3953,6 +4543,9 @@
       <c r="D197" t="inlineStr"/>
       <c r="E197" t="inlineStr"/>
       <c r="F197" t="inlineStr"/>
+      <c r="G197" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="n">
@@ -3973,6 +4566,9 @@
       <c r="F198" t="n">
         <v>24.9</v>
       </c>
+      <c r="G198" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="n">
@@ -3993,6 +4589,9 @@
       <c r="F199" t="n">
         <v>24.9</v>
       </c>
+      <c r="G199" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="n">
@@ -4007,6 +4606,9 @@
       <c r="D200" t="inlineStr"/>
       <c r="E200" t="inlineStr"/>
       <c r="F200" t="inlineStr"/>
+      <c r="G200" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="n">
@@ -4021,6 +4623,9 @@
       <c r="D201" t="inlineStr"/>
       <c r="E201" t="inlineStr"/>
       <c r="F201" t="inlineStr"/>
+      <c r="G201" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
@@ -4041,6 +4646,9 @@
       <c r="F202" t="n">
         <v>25.3</v>
       </c>
+      <c r="G202" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="n">
@@ -4061,6 +4669,9 @@
       <c r="F203" t="n">
         <v>25.3</v>
       </c>
+      <c r="G203" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="n">
@@ -4075,6 +4686,9 @@
       <c r="D204" t="inlineStr"/>
       <c r="E204" t="inlineStr"/>
       <c r="F204" t="inlineStr"/>
+      <c r="G204" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="n">
@@ -4089,6 +4703,9 @@
       <c r="D205" t="inlineStr"/>
       <c r="E205" t="inlineStr"/>
       <c r="F205" t="inlineStr"/>
+      <c r="G205" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="n">
@@ -4109,6 +4726,9 @@
       <c r="F206" t="n">
         <v>24.4</v>
       </c>
+      <c r="G206" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="n">
@@ -4129,6 +4749,9 @@
       <c r="F207" t="n">
         <v>24.9</v>
       </c>
+      <c r="G207" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="n">
@@ -4149,6 +4772,9 @@
       <c r="F208" t="n">
         <v>24.9</v>
       </c>
+      <c r="G208" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="n">
@@ -4169,6 +4795,9 @@
       <c r="F209" t="n">
         <v>24.9</v>
       </c>
+      <c r="G209" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="n">
@@ -4189,6 +4818,9 @@
       <c r="F210" t="n">
         <v>24.9</v>
       </c>
+      <c r="G210" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="n">
@@ -4209,6 +4841,9 @@
       <c r="F211" t="n">
         <v>24.9</v>
       </c>
+      <c r="G211" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="n">
@@ -4229,6 +4864,9 @@
       <c r="F212" t="n">
         <v>24.9</v>
       </c>
+      <c r="G212" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="n">
@@ -4243,6 +4881,9 @@
       <c r="D213" t="inlineStr"/>
       <c r="E213" t="inlineStr"/>
       <c r="F213" t="inlineStr"/>
+      <c r="G213" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="n">
@@ -4257,6 +4898,9 @@
       <c r="D214" t="inlineStr"/>
       <c r="E214" t="inlineStr"/>
       <c r="F214" t="inlineStr"/>
+      <c r="G214" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="n">
@@ -4277,6 +4921,9 @@
       <c r="F215" t="n">
         <v>21.4</v>
       </c>
+      <c r="G215" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="n">
@@ -4297,6 +4944,9 @@
       <c r="F216" t="n">
         <v>21.4</v>
       </c>
+      <c r="G216" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
@@ -4317,6 +4967,9 @@
       <c r="F217" t="n">
         <v>25.4</v>
       </c>
+      <c r="G217" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="n">
@@ -4337,6 +4990,9 @@
       <c r="F218" t="n">
         <v>25.4</v>
       </c>
+      <c r="G218" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="n">
@@ -4351,6 +5007,9 @@
       <c r="D219" t="inlineStr"/>
       <c r="E219" t="inlineStr"/>
       <c r="F219" t="inlineStr"/>
+      <c r="G219" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="n">
@@ -4365,6 +5024,9 @@
       <c r="D220" t="inlineStr"/>
       <c r="E220" t="inlineStr"/>
       <c r="F220" t="inlineStr"/>
+      <c r="G220" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="n">
@@ -4385,6 +5047,9 @@
       <c r="F221" t="n">
         <v>25.6</v>
       </c>
+      <c r="G221" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="n">
@@ -4405,6 +5070,9 @@
       <c r="F222" t="n">
         <v>25.6</v>
       </c>
+      <c r="G222" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="n">
@@ -4423,6 +5091,9 @@
       <c r="F223" t="n">
         <v>19.2</v>
       </c>
+      <c r="G223" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="n">
@@ -4437,6 +5108,9 @@
       <c r="D224" t="inlineStr"/>
       <c r="E224" t="inlineStr"/>
       <c r="F224" t="inlineStr"/>
+      <c r="G224" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="n">
@@ -4457,6 +5131,9 @@
       <c r="F225" t="n">
         <v>25.4</v>
       </c>
+      <c r="G225" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="n">
@@ -4477,6 +5154,9 @@
       <c r="F226" t="n">
         <v>25.4</v>
       </c>
+      <c r="G226" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="n">
@@ -4491,6 +5171,9 @@
       <c r="D227" t="inlineStr"/>
       <c r="E227" t="inlineStr"/>
       <c r="F227" t="inlineStr"/>
+      <c r="G227" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="n">
@@ -4511,6 +5194,9 @@
       <c r="F228" t="n">
         <v>24</v>
       </c>
+      <c r="G228" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="n">
@@ -4525,6 +5211,9 @@
       <c r="D229" t="inlineStr"/>
       <c r="E229" t="inlineStr"/>
       <c r="F229" t="inlineStr"/>
+      <c r="G229" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="n">
@@ -4545,6 +5234,9 @@
       <c r="F230" t="n">
         <v>24</v>
       </c>
+      <c r="G230" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="n">
@@ -4561,6 +5253,9 @@
       </c>
       <c r="E231" t="inlineStr"/>
       <c r="F231" t="inlineStr"/>
+      <c r="G231" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="n">
@@ -4575,6 +5270,9 @@
       <c r="D232" t="inlineStr"/>
       <c r="E232" t="inlineStr"/>
       <c r="F232" t="inlineStr"/>
+      <c r="G232" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="n">
@@ -4595,6 +5293,9 @@
       <c r="F233" t="n">
         <v>26.1</v>
       </c>
+      <c r="G233" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="n">
@@ -4615,6 +5316,9 @@
       <c r="F234" t="n">
         <v>26.1</v>
       </c>
+      <c r="G234" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="n">
@@ -4635,6 +5339,9 @@
       <c r="F235" t="n">
         <v>26</v>
       </c>
+      <c r="G235" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="n">
@@ -4655,6 +5362,9 @@
       <c r="F236" t="n">
         <v>26</v>
       </c>
+      <c r="G236" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="n">
@@ -4675,6 +5385,9 @@
       <c r="F237" t="n">
         <v>26</v>
       </c>
+      <c r="G237" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="n">
@@ -4695,6 +5408,9 @@
       <c r="F238" t="n">
         <v>26</v>
       </c>
+      <c r="G238" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="n">
@@ -4715,6 +5431,9 @@
       <c r="F239" t="n">
         <v>26</v>
       </c>
+      <c r="G239" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="n">
@@ -4735,6 +5454,9 @@
       <c r="F240" t="n">
         <v>26</v>
       </c>
+      <c r="G240" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="n">
@@ -4755,6 +5477,9 @@
       <c r="F241" t="n">
         <v>26</v>
       </c>
+      <c r="G241" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="n">
@@ -4775,6 +5500,9 @@
       <c r="F242" t="n">
         <v>26</v>
       </c>
+      <c r="G242" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="n">
@@ -4789,6 +5517,9 @@
       <c r="D243" t="inlineStr"/>
       <c r="E243" t="inlineStr"/>
       <c r="F243" t="inlineStr"/>
+      <c r="G243" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="n">
@@ -4803,6 +5534,9 @@
       <c r="D244" t="inlineStr"/>
       <c r="E244" t="inlineStr"/>
       <c r="F244" t="inlineStr"/>
+      <c r="G244" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="n">
@@ -4823,6 +5557,9 @@
       <c r="F245" t="n">
         <v>26</v>
       </c>
+      <c r="G245" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="n">
@@ -4843,6 +5580,9 @@
       <c r="F246" t="n">
         <v>26</v>
       </c>
+      <c r="G246" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="n">
@@ -4857,6 +5597,9 @@
       <c r="D247" t="inlineStr"/>
       <c r="E247" t="inlineStr"/>
       <c r="F247" t="inlineStr"/>
+      <c r="G247" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="n">
@@ -4871,6 +5614,9 @@
       <c r="D248" t="inlineStr"/>
       <c r="E248" t="inlineStr"/>
       <c r="F248" t="inlineStr"/>
+      <c r="G248" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="n">
@@ -4891,6 +5637,9 @@
       <c r="F249" t="n">
         <v>26.8</v>
       </c>
+      <c r="G249" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
@@ -4911,6 +5660,9 @@
       <c r="F250" t="n">
         <v>26.8</v>
       </c>
+      <c r="G250" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="n">
@@ -4925,6 +5677,9 @@
       <c r="D251" t="inlineStr"/>
       <c r="E251" t="inlineStr"/>
       <c r="F251" t="inlineStr"/>
+      <c r="G251" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="n">
@@ -4939,6 +5694,9 @@
       <c r="D252" t="inlineStr"/>
       <c r="E252" t="inlineStr"/>
       <c r="F252" t="inlineStr"/>
+      <c r="G252" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="n">
@@ -4953,6 +5711,9 @@
       <c r="D253" t="inlineStr"/>
       <c r="E253" t="inlineStr"/>
       <c r="F253" t="inlineStr"/>
+      <c r="G253" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="n">
@@ -4973,6 +5734,9 @@
       <c r="F254" t="n">
         <v>25.3</v>
       </c>
+      <c r="G254" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="n">
@@ -4987,6 +5751,9 @@
       <c r="D255" t="inlineStr"/>
       <c r="E255" t="inlineStr"/>
       <c r="F255" t="inlineStr"/>
+      <c r="G255" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="n">
@@ -5001,6 +5768,9 @@
       <c r="D256" t="inlineStr"/>
       <c r="E256" t="inlineStr"/>
       <c r="F256" t="inlineStr"/>
+      <c r="G256" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="n">
@@ -5021,6 +5791,9 @@
       <c r="F257" t="n">
         <v>26.5</v>
       </c>
+      <c r="G257" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="n">
@@ -5041,6 +5814,9 @@
       <c r="F258" t="n">
         <v>26.5</v>
       </c>
+      <c r="G258" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="n">
@@ -5055,6 +5831,9 @@
       <c r="D259" t="inlineStr"/>
       <c r="E259" t="inlineStr"/>
       <c r="F259" t="inlineStr"/>
+      <c r="G259" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="n">
@@ -5069,6 +5848,9 @@
       <c r="D260" t="inlineStr"/>
       <c r="E260" t="inlineStr"/>
       <c r="F260" t="inlineStr"/>
+      <c r="G260" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="n">
@@ -5089,6 +5871,9 @@
       <c r="F261" t="n">
         <v>26.5</v>
       </c>
+      <c r="G261" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="n">
@@ -5109,6 +5894,9 @@
       <c r="F262" t="n">
         <v>26.5</v>
       </c>
+      <c r="G262" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="n">
@@ -5123,6 +5911,9 @@
       <c r="D263" t="inlineStr"/>
       <c r="E263" t="inlineStr"/>
       <c r="F263" t="inlineStr"/>
+      <c r="G263" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="n">
@@ -5137,6 +5928,9 @@
       <c r="D264" t="inlineStr"/>
       <c r="E264" t="inlineStr"/>
       <c r="F264" t="inlineStr"/>
+      <c r="G264" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="n">
@@ -5157,6 +5951,9 @@
       <c r="F265" t="n">
         <v>27.5</v>
       </c>
+      <c r="G265" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="n">
@@ -5177,6 +5974,9 @@
       <c r="F266" t="n">
         <v>27.5</v>
       </c>
+      <c r="G266" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="n">
@@ -5191,6 +5991,9 @@
       <c r="D267" t="inlineStr"/>
       <c r="E267" t="inlineStr"/>
       <c r="F267" t="inlineStr"/>
+      <c r="G267" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="n">
@@ -5211,6 +6014,9 @@
       <c r="F268" t="n">
         <v>26.3</v>
       </c>
+      <c r="G268" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="n">
@@ -5231,6 +6037,9 @@
       <c r="F269" t="n">
         <v>26.3</v>
       </c>
+      <c r="G269" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="n">
@@ -5251,6 +6060,9 @@
       <c r="F270" t="n">
         <v>26.6</v>
       </c>
+      <c r="G270" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="n">
@@ -5265,6 +6077,9 @@
       <c r="D271" t="inlineStr"/>
       <c r="E271" t="inlineStr"/>
       <c r="F271" t="inlineStr"/>
+      <c r="G271" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="n">
@@ -5279,6 +6094,9 @@
       <c r="D272" t="inlineStr"/>
       <c r="E272" t="inlineStr"/>
       <c r="F272" t="inlineStr"/>
+      <c r="G272" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="n">
@@ -5299,6 +6117,9 @@
       <c r="F273" t="n">
         <v>26.6</v>
       </c>
+      <c r="G273" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="n">
@@ -5319,6 +6140,9 @@
       <c r="F274" t="n">
         <v>26.6</v>
       </c>
+      <c r="G274" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="n">
@@ -5339,6 +6163,9 @@
       <c r="F275" t="n">
         <v>26.6</v>
       </c>
+      <c r="G275" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="n">
@@ -5359,6 +6186,9 @@
       <c r="F276" t="n">
         <v>26.6</v>
       </c>
+      <c r="G276" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="n">
@@ -5379,6 +6209,9 @@
       <c r="F277" t="n">
         <v>26.6</v>
       </c>
+      <c r="G277" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="n">
@@ -5399,6 +6232,9 @@
       <c r="F278" t="n">
         <v>26.6</v>
       </c>
+      <c r="G278" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="n">
@@ -5419,6 +6255,9 @@
       <c r="F279" t="n">
         <v>26.6</v>
       </c>
+      <c r="G279" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="n">
@@ -5439,6 +6278,9 @@
       <c r="F280" t="n">
         <v>26.6</v>
       </c>
+      <c r="G280" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="n">
@@ -5459,6 +6301,9 @@
       <c r="F281" t="n">
         <v>26.6</v>
       </c>
+      <c r="G281" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="n">
@@ -5479,6 +6324,9 @@
       <c r="F282" t="n">
         <v>26.6</v>
       </c>
+      <c r="G282" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="n">
@@ -5493,6 +6341,9 @@
       <c r="D283" t="inlineStr"/>
       <c r="E283" t="inlineStr"/>
       <c r="F283" t="inlineStr"/>
+      <c r="G283" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="n">
@@ -5507,6 +6358,9 @@
       <c r="D284" t="inlineStr"/>
       <c r="E284" t="inlineStr"/>
       <c r="F284" t="inlineStr"/>
+      <c r="G284" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="n">
@@ -5527,6 +6381,9 @@
       <c r="F285" t="n">
         <v>27.1</v>
       </c>
+      <c r="G285" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="n">
@@ -5547,6 +6404,9 @@
       <c r="F286" t="n">
         <v>27.1</v>
       </c>
+      <c r="G286" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="n">
@@ -5561,6 +6421,9 @@
       <c r="D287" t="inlineStr"/>
       <c r="E287" t="inlineStr"/>
       <c r="F287" t="inlineStr"/>
+      <c r="G287" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="n">
@@ -5575,6 +6438,9 @@
       <c r="D288" t="inlineStr"/>
       <c r="E288" t="inlineStr"/>
       <c r="F288" t="inlineStr"/>
+      <c r="G288" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="n">
@@ -5595,6 +6461,9 @@
       <c r="F289" t="n">
         <v>27.1</v>
       </c>
+      <c r="G289" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="n">
@@ -5615,6 +6484,9 @@
       <c r="F290" t="n">
         <v>27.1</v>
       </c>
+      <c r="G290" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="n">
@@ -5629,6 +6501,9 @@
       <c r="D291" t="inlineStr"/>
       <c r="E291" t="inlineStr"/>
       <c r="F291" t="inlineStr"/>
+      <c r="G291" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="n">
@@ -5645,6 +6520,9 @@
       </c>
       <c r="E292" t="inlineStr"/>
       <c r="F292" t="inlineStr"/>
+      <c r="G292" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="n">
@@ -5659,6 +6537,9 @@
       <c r="D293" t="inlineStr"/>
       <c r="E293" t="inlineStr"/>
       <c r="F293" t="inlineStr"/>
+      <c r="G293" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="n">
@@ -5673,6 +6554,9 @@
       <c r="D294" t="inlineStr"/>
       <c r="E294" t="inlineStr"/>
       <c r="F294" t="inlineStr"/>
+      <c r="G294" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="n">
@@ -5687,6 +6571,9 @@
       <c r="D295" t="inlineStr"/>
       <c r="E295" t="inlineStr"/>
       <c r="F295" t="inlineStr"/>
+      <c r="G295" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="n">
@@ -5707,6 +6594,9 @@
       <c r="F296" t="n">
         <v>26.8</v>
       </c>
+      <c r="G296" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="n">
@@ -5727,6 +6617,9 @@
       <c r="F297" t="n">
         <v>27.8</v>
       </c>
+      <c r="G297" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="n">
@@ -5747,6 +6640,9 @@
       <c r="F298" t="n">
         <v>27.8</v>
       </c>
+      <c r="G298" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="n">
@@ -5767,6 +6663,9 @@
       <c r="F299" t="n">
         <v>27.8</v>
       </c>
+      <c r="G299" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="n">
@@ -5781,6 +6680,9 @@
       <c r="D300" t="inlineStr"/>
       <c r="E300" t="inlineStr"/>
       <c r="F300" t="inlineStr"/>
+      <c r="G300" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="n">
@@ -5801,6 +6703,9 @@
       <c r="F301" t="n">
         <v>25.8</v>
       </c>
+      <c r="G301" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="n">
@@ -5821,6 +6726,9 @@
       <c r="F302" t="n">
         <v>25.8</v>
       </c>
+      <c r="G302" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="n">
@@ -5841,6 +6749,9 @@
       <c r="F303" t="n">
         <v>25.8</v>
       </c>
+      <c r="G303" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="n">
@@ -5855,6 +6766,9 @@
       <c r="D304" t="inlineStr"/>
       <c r="E304" t="inlineStr"/>
       <c r="F304" t="inlineStr"/>
+      <c r="G304" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="n">
@@ -5875,6 +6789,9 @@
       <c r="F305" t="n">
         <v>27.1</v>
       </c>
+      <c r="G305" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="n">
@@ -5895,6 +6812,9 @@
       <c r="F306" t="n">
         <v>27.1</v>
       </c>
+      <c r="G306" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="n">
@@ -5909,6 +6829,9 @@
       <c r="D307" t="inlineStr"/>
       <c r="E307" t="inlineStr"/>
       <c r="F307" t="inlineStr"/>
+      <c r="G307" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="n">
@@ -5923,6 +6846,9 @@
       <c r="D308" t="inlineStr"/>
       <c r="E308" t="inlineStr"/>
       <c r="F308" t="inlineStr"/>
+      <c r="G308" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="n">
@@ -5943,6 +6869,9 @@
       <c r="F309" t="n">
         <v>25.3</v>
       </c>
+      <c r="G309" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="n">
@@ -5963,6 +6892,9 @@
       <c r="F310" t="n">
         <v>25.3</v>
       </c>
+      <c r="G310" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="n">
@@ -5983,6 +6915,9 @@
       <c r="F311" t="n">
         <v>25.3</v>
       </c>
+      <c r="G311" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="n">
@@ -6003,6 +6938,9 @@
       <c r="F312" t="n">
         <v>25.4</v>
       </c>
+      <c r="G312" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="n">
@@ -6017,6 +6955,9 @@
       <c r="D313" t="inlineStr"/>
       <c r="E313" t="inlineStr"/>
       <c r="F313" t="inlineStr"/>
+      <c r="G313" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="n">
@@ -6031,6 +6972,9 @@
       <c r="D314" t="inlineStr"/>
       <c r="E314" t="inlineStr"/>
       <c r="F314" t="inlineStr"/>
+      <c r="G314" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="n">
@@ -6051,6 +6995,9 @@
       <c r="F315" t="n">
         <v>26.3</v>
       </c>
+      <c r="G315" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="n">
@@ -6071,6 +7018,9 @@
       <c r="F316" t="n">
         <v>26.3</v>
       </c>
+      <c r="G316" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="n">
@@ -6091,6 +7041,9 @@
       <c r="F317" t="n">
         <v>25.1</v>
       </c>
+      <c r="G317" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="n">
@@ -6111,6 +7064,9 @@
       <c r="F318" t="n">
         <v>25.1</v>
       </c>
+      <c r="G318" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="n">
@@ -6125,6 +7081,9 @@
       <c r="D319" t="inlineStr"/>
       <c r="E319" t="inlineStr"/>
       <c r="F319" t="inlineStr"/>
+      <c r="G319" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="n">
@@ -6139,6 +7098,9 @@
       <c r="D320" t="inlineStr"/>
       <c r="E320" t="inlineStr"/>
       <c r="F320" t="inlineStr"/>
+      <c r="G320" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="n">
@@ -6159,6 +7121,9 @@
       <c r="F321" t="n">
         <v>26.8</v>
       </c>
+      <c r="G321" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="n">
@@ -6179,6 +7144,9 @@
       <c r="F322" t="n">
         <v>26.8</v>
       </c>
+      <c r="G322" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="n">
@@ -6199,6 +7167,9 @@
       <c r="F323" t="n">
         <v>26.8</v>
       </c>
+      <c r="G323" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="n">
@@ -6219,6 +7190,9 @@
       <c r="F324" t="n">
         <v>26.8</v>
       </c>
+      <c r="G324" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="n">
@@ -6239,6 +7213,9 @@
       <c r="F325" t="n">
         <v>26.8</v>
       </c>
+      <c r="G325" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="n">
@@ -6259,6 +7236,9 @@
       <c r="F326" t="n">
         <v>26.8</v>
       </c>
+      <c r="G326" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="n">
@@ -6279,6 +7259,9 @@
       <c r="F327" t="n">
         <v>26.8</v>
       </c>
+      <c r="G327" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="n">
@@ -6299,6 +7282,9 @@
       <c r="F328" t="n">
         <v>26.8</v>
       </c>
+      <c r="G328" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="329">
       <c r="A329" s="1" t="n">
@@ -6313,6 +7299,9 @@
       <c r="D329" t="inlineStr"/>
       <c r="E329" t="inlineStr"/>
       <c r="F329" t="inlineStr"/>
+      <c r="G329" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="330">
       <c r="A330" s="1" t="n">
@@ -6333,6 +7322,9 @@
       <c r="F330" t="n">
         <v>26.8</v>
       </c>
+      <c r="G330" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="331">
       <c r="A331" s="1" t="n">
@@ -6353,6 +7345,9 @@
       <c r="F331" t="n">
         <v>26.8</v>
       </c>
+      <c r="G331" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="332">
       <c r="A332" s="1" t="n">
@@ -6367,6 +7362,9 @@
       <c r="D332" t="inlineStr"/>
       <c r="E332" t="inlineStr"/>
       <c r="F332" t="inlineStr"/>
+      <c r="G332" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="333">
       <c r="A333" s="1" t="n">
@@ -6381,6 +7379,9 @@
       <c r="D333" t="inlineStr"/>
       <c r="E333" t="inlineStr"/>
       <c r="F333" t="inlineStr"/>
+      <c r="G333" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="334">
       <c r="A334" s="1" t="n">
@@ -6395,6 +7396,9 @@
       <c r="D334" t="inlineStr"/>
       <c r="E334" t="inlineStr"/>
       <c r="F334" t="inlineStr"/>
+      <c r="G334" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="335">
       <c r="A335" s="1" t="n">
@@ -6409,6 +7413,9 @@
       <c r="D335" t="inlineStr"/>
       <c r="E335" t="inlineStr"/>
       <c r="F335" t="inlineStr"/>
+      <c r="G335" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="336">
       <c r="A336" s="1" t="n">
@@ -6423,6 +7430,9 @@
       <c r="D336" t="inlineStr"/>
       <c r="E336" t="inlineStr"/>
       <c r="F336" t="inlineStr"/>
+      <c r="G336" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="337">
       <c r="A337" s="1" t="n">
@@ -6437,6 +7447,9 @@
       <c r="D337" t="inlineStr"/>
       <c r="E337" t="inlineStr"/>
       <c r="F337" t="inlineStr"/>
+      <c r="G337" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="338">
       <c r="A338" s="1" t="n">
@@ -6457,6 +7470,9 @@
       <c r="F338" t="n">
         <v>27.3</v>
       </c>
+      <c r="G338" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="339">
       <c r="A339" s="1" t="n">
@@ -6477,6 +7493,9 @@
       <c r="F339" t="n">
         <v>27.3</v>
       </c>
+      <c r="G339" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="340">
       <c r="A340" s="1" t="n">
@@ -6491,6 +7510,9 @@
       <c r="D340" t="inlineStr"/>
       <c r="E340" t="inlineStr"/>
       <c r="F340" t="inlineStr"/>
+      <c r="G340" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="341">
       <c r="A341" s="1" t="n">
@@ -6505,6 +7527,9 @@
       <c r="D341" t="inlineStr"/>
       <c r="E341" t="inlineStr"/>
       <c r="F341" t="inlineStr"/>
+      <c r="G341" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="342">
       <c r="A342" s="1" t="n">
@@ -6525,6 +7550,9 @@
       <c r="F342" t="n">
         <v>27.1</v>
       </c>
+      <c r="G342" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="343">
       <c r="A343" s="1" t="n">
@@ -6545,6 +7573,9 @@
       <c r="F343" t="n">
         <v>27.1</v>
       </c>
+      <c r="G343" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="344">
       <c r="A344" s="1" t="n">
@@ -6565,6 +7596,9 @@
       <c r="F344" t="n">
         <v>22.7</v>
       </c>
+      <c r="G344" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="345">
       <c r="A345" s="1" t="n">
@@ -6579,6 +7613,9 @@
       <c r="D345" t="inlineStr"/>
       <c r="E345" t="inlineStr"/>
       <c r="F345" t="inlineStr"/>
+      <c r="G345" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="346">
       <c r="A346" s="1" t="n">
@@ -6599,6 +7636,9 @@
       <c r="F346" t="n">
         <v>27.3</v>
       </c>
+      <c r="G346" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="347">
       <c r="A347" s="1" t="n">
@@ -6619,6 +7659,9 @@
       <c r="F347" t="n">
         <v>27.3</v>
       </c>
+      <c r="G347" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="348">
       <c r="A348" s="1" t="n">
@@ -6633,6 +7676,9 @@
       <c r="D348" t="inlineStr"/>
       <c r="E348" t="inlineStr"/>
       <c r="F348" t="inlineStr"/>
+      <c r="G348" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="349">
       <c r="A349" s="1" t="n">
@@ -6653,6 +7699,9 @@
       <c r="F349" t="n">
         <v>24.4</v>
       </c>
+      <c r="G349" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="350">
       <c r="A350" s="1" t="n">
@@ -6673,6 +7722,9 @@
       <c r="F350" t="n">
         <v>24.4</v>
       </c>
+      <c r="G350" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="351">
       <c r="A351" s="1" t="n">
@@ -6687,6 +7739,9 @@
       <c r="D351" t="inlineStr"/>
       <c r="E351" t="inlineStr"/>
       <c r="F351" t="inlineStr"/>
+      <c r="G351" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="352">
       <c r="A352" s="1" t="n">
@@ -6701,6 +7756,9 @@
       <c r="D352" t="inlineStr"/>
       <c r="E352" t="inlineStr"/>
       <c r="F352" t="inlineStr"/>
+      <c r="G352" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="353">
       <c r="A353" s="1" t="n">
@@ -6721,6 +7779,9 @@
       <c r="F353" t="n">
         <v>27.8</v>
       </c>
+      <c r="G353" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="354">
       <c r="A354" s="1" t="n">
@@ -6741,6 +7802,9 @@
       <c r="F354" t="n">
         <v>27.8</v>
       </c>
+      <c r="G354" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="355">
       <c r="A355" s="1" t="n">
@@ -6761,6 +7825,9 @@
       <c r="F355" t="n">
         <v>27.8</v>
       </c>
+      <c r="G355" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="356">
       <c r="A356" s="1" t="n">
@@ -6781,6 +7848,9 @@
       <c r="F356" t="n">
         <v>27.8</v>
       </c>
+      <c r="G356" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="357">
       <c r="A357" s="1" t="n">
@@ -6801,6 +7871,9 @@
       <c r="F357" t="n">
         <v>27.8</v>
       </c>
+      <c r="G357" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="358">
       <c r="A358" s="1" t="n">
@@ -6821,6 +7894,9 @@
       <c r="F358" t="n">
         <v>27.8</v>
       </c>
+      <c r="G358" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="359">
       <c r="A359" s="1" t="n">
@@ -6835,6 +7911,9 @@
       <c r="D359" t="inlineStr"/>
       <c r="E359" t="inlineStr"/>
       <c r="F359" t="inlineStr"/>
+      <c r="G359" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="360">
       <c r="A360" s="1" t="n">
@@ -6849,6 +7928,9 @@
       <c r="D360" t="inlineStr"/>
       <c r="E360" t="inlineStr"/>
       <c r="F360" t="inlineStr"/>
+      <c r="G360" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="361">
       <c r="A361" s="1" t="n">
@@ -6869,6 +7951,9 @@
       <c r="F361" t="n">
         <v>24.6</v>
       </c>
+      <c r="G361" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="362">
       <c r="A362" s="1" t="n">
@@ -6887,6 +7972,9 @@
         <v>24.9</v>
       </c>
       <c r="F362" t="inlineStr"/>
+      <c r="G362" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="363">
       <c r="A363" s="1" t="n">
@@ -6901,6 +7989,9 @@
       <c r="D363" t="inlineStr"/>
       <c r="E363" t="inlineStr"/>
       <c r="F363" t="inlineStr"/>
+      <c r="G363" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="364">
       <c r="A364" s="1" t="n">
@@ -6921,6 +8012,9 @@
       <c r="F364" t="n">
         <v>28.1</v>
       </c>
+      <c r="G364" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="365">
       <c r="A365" s="1" t="n">
@@ -6941,6 +8035,9 @@
       <c r="F365" t="n">
         <v>28.1</v>
       </c>
+      <c r="G365" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="366">
       <c r="A366" s="1" t="n">
@@ -6955,6 +8052,9 @@
       <c r="D366" t="inlineStr"/>
       <c r="E366" t="inlineStr"/>
       <c r="F366" t="inlineStr"/>
+      <c r="G366" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="367">
       <c r="A367" s="1" t="n">
@@ -6969,6 +8069,9 @@
       <c r="D367" t="inlineStr"/>
       <c r="E367" t="inlineStr"/>
       <c r="F367" t="inlineStr"/>
+      <c r="G367" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="368">
       <c r="A368" s="1" t="n">
@@ -6989,6 +8092,9 @@
       <c r="F368" t="n">
         <v>26.8</v>
       </c>
+      <c r="G368" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="369">
       <c r="A369" s="1" t="n">
@@ -7009,6 +8115,9 @@
       <c r="F369" t="n">
         <v>26.8</v>
       </c>
+      <c r="G369" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="370">
       <c r="A370" s="1" t="n">
@@ -7023,6 +8132,9 @@
       <c r="D370" t="inlineStr"/>
       <c r="E370" t="inlineStr"/>
       <c r="F370" t="inlineStr"/>
+      <c r="G370" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="371">
       <c r="A371" s="1" t="n">
@@ -7037,6 +8149,9 @@
       <c r="D371" t="inlineStr"/>
       <c r="E371" t="inlineStr"/>
       <c r="F371" t="inlineStr"/>
+      <c r="G371" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="372">
       <c r="A372" s="1" t="n">
@@ -7057,6 +8172,9 @@
       <c r="F372" t="n">
         <v>26.5</v>
       </c>
+      <c r="G372" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="373">
       <c r="A373" s="1" t="n">
@@ -7077,6 +8195,9 @@
       <c r="F373" t="n">
         <v>26.5</v>
       </c>
+      <c r="G373" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="374">
       <c r="A374" s="1" t="n">
@@ -7091,6 +8212,9 @@
       <c r="D374" t="inlineStr"/>
       <c r="E374" t="inlineStr"/>
       <c r="F374" t="inlineStr"/>
+      <c r="G374" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="375">
       <c r="A375" s="1" t="n">
@@ -7111,6 +8235,9 @@
       <c r="F375" t="n">
         <v>25.4</v>
       </c>
+      <c r="G375" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="376">
       <c r="A376" s="1" t="n">
@@ -7131,6 +8258,9 @@
       <c r="F376" t="n">
         <v>25.4</v>
       </c>
+      <c r="G376" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="377">
       <c r="A377" s="1" t="n">
@@ -7149,6 +8279,9 @@
         <v>24.9</v>
       </c>
       <c r="F377" t="inlineStr"/>
+      <c r="G377" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="378">
       <c r="A378" s="1" t="n">
@@ -7163,6 +8296,9 @@
       <c r="D378" t="inlineStr"/>
       <c r="E378" t="inlineStr"/>
       <c r="F378" t="inlineStr"/>
+      <c r="G378" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="379">
       <c r="A379" s="1" t="n">
@@ -7183,6 +8319,9 @@
       <c r="F379" t="n">
         <v>27</v>
       </c>
+      <c r="G379" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="380">
       <c r="A380" s="1" t="n">
@@ -7203,6 +8342,9 @@
       <c r="F380" t="n">
         <v>27</v>
       </c>
+      <c r="G380" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="381">
       <c r="A381" s="1" t="n">
@@ -7217,6 +8359,9 @@
       <c r="D381" t="inlineStr"/>
       <c r="E381" t="inlineStr"/>
       <c r="F381" t="inlineStr"/>
+      <c r="G381" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="382">
       <c r="A382" s="1" t="n">
@@ -7231,6 +8376,9 @@
       <c r="D382" t="inlineStr"/>
       <c r="E382" t="inlineStr"/>
       <c r="F382" t="inlineStr"/>
+      <c r="G382" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="383">
       <c r="A383" s="1" t="n">
@@ -7251,6 +8399,9 @@
       <c r="F383" t="n">
         <v>26.8</v>
       </c>
+      <c r="G383" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="384">
       <c r="A384" s="1" t="n">
@@ -7270,6 +8421,9 @@
       </c>
       <c r="F384" t="n">
         <v>26.8</v>
+      </c>
+      <c r="G384" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>